<commit_message>
Updated database with one more intent Created function to chatbot
</commit_message>
<xml_diff>
--- a/chatbot/training_chatbot.xlsx
+++ b/chatbot/training_chatbot.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimmy\Desktop\Copia_de_Seguridad\Keepcoding_2\TFB-SmartBot\chatbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataScience\Machine Learning\Projects\Keepcoding\TFB\TFB-SmartBot\chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24FD3D5-0F77-4BE2-BEF1-5BEC71767A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B1C6C3-88B8-4EA4-A292-2A6DB79FB31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E701B219-9CB5-4FB1-A8B1-D6439049C12F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E701B219-9CB5-4FB1-A8B1-D6439049C12F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$1:$B$83</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="114">
   <si>
     <t>Intent type</t>
   </si>
@@ -232,6 +235,150 @@
   </si>
   <si>
     <t>Greeting</t>
+  </si>
+  <si>
+    <t>How’re you?</t>
+  </si>
+  <si>
+    <t>How you doing?</t>
+  </si>
+  <si>
+    <t>How you doin'?</t>
+  </si>
+  <si>
+    <t>How is everything?</t>
+  </si>
+  <si>
+    <t>How’s everything going?</t>
+  </si>
+  <si>
+    <t>How it's going?</t>
+  </si>
+  <si>
+    <t>How are things?</t>
+  </si>
+  <si>
+    <t>How are things with you?</t>
+  </si>
+  <si>
+    <t>What’s happening?</t>
+  </si>
+  <si>
+    <t>It has been a long time.</t>
+  </si>
+  <si>
+    <t>It’s always a pleasure to see you.</t>
+  </si>
+  <si>
+    <t>Could you tell me about cryptocurrencies?</t>
+  </si>
+  <si>
+    <t>I wonder if you could explain what is socialism</t>
+  </si>
+  <si>
+    <t>I wonder if you could tell me information on Machine Learning</t>
+  </si>
+  <si>
+    <t>I wanna know everything about Psychology</t>
+  </si>
+  <si>
+    <t>I wanna know how a computer works</t>
+  </si>
+  <si>
+    <t>Please, search info about Johnny Depp</t>
+  </si>
+  <si>
+    <t>I want to know more about it</t>
+  </si>
+  <si>
+    <t>What topics are related to Data Science?</t>
+  </si>
+  <si>
+    <t>I wanna know more about Bitcoin</t>
+  </si>
+  <si>
+    <t>Tell me things connected to aerospace engineering</t>
+  </si>
+  <si>
+    <t>Tell me things connected to cinema</t>
+  </si>
+  <si>
+    <t>What can you tell me connected to electric guitar?</t>
+  </si>
+  <si>
+    <t>Suggest me topics connected to apple</t>
+  </si>
+  <si>
+    <t>tell me things connected to instagram</t>
+  </si>
+  <si>
+    <t>Suggest me words connected to Lolita</t>
+  </si>
+  <si>
+    <t>Give me topics connected to stand-up comedy</t>
+  </si>
+  <si>
+    <t>What topics are connected to Data Science?</t>
+  </si>
+  <si>
+    <t>Tell me things linked to aerospace engineering</t>
+  </si>
+  <si>
+    <t>Tell me things linked to cinema</t>
+  </si>
+  <si>
+    <t>What can you tell me linked to electric guitar?</t>
+  </si>
+  <si>
+    <t>Suggest me topics linked to apple</t>
+  </si>
+  <si>
+    <t>tell me things linked to instagram</t>
+  </si>
+  <si>
+    <t>Suggest me words linked to Lolita</t>
+  </si>
+  <si>
+    <t>Give me topics linked to stand-up comedy</t>
+  </si>
+  <si>
+    <t>What topics are linked to Data Science?</t>
+  </si>
+  <si>
+    <t>Farewell</t>
+  </si>
+  <si>
+    <t>Goodbye</t>
+  </si>
+  <si>
+    <t>See you!</t>
+  </si>
+  <si>
+    <t>See ya</t>
+  </si>
+  <si>
+    <t>Bye, bye</t>
+  </si>
+  <si>
+    <t>I’ve gotta go </t>
+  </si>
+  <si>
+    <t>See you later</t>
+  </si>
+  <si>
+    <t>Laters</t>
+  </si>
+  <si>
+    <t>Catch ya later</t>
+  </si>
+  <si>
+    <t>Take it easy!</t>
+  </si>
+  <si>
+    <t>Ciao</t>
+  </si>
+  <si>
+    <t>Cheerio</t>
   </si>
 </sst>
 </file>
@@ -583,18 +730,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8947F2DF-9E18-4EF9-8E6E-53A318233C25}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -610,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -618,7 +765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -626,7 +773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -634,7 +781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -642,7 +789,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -650,7 +797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -658,7 +805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -666,7 +813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -674,7 +821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -682,7 +829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -690,7 +837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -698,7 +845,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -706,7 +853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -714,7 +861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -722,7 +869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -730,7 +877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -738,7 +885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -746,7 +893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -754,143 +901,143 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>21</v>
       </c>
@@ -898,207 +1045,584 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>21</v>
       </c>
       <c r="B39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>42</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>42</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>42</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>42</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>42</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>42</v>
+      </c>
+      <c r="B78" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B79" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>42</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>42</v>
+      </c>
+      <c r="B92" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>42</v>
+      </c>
+      <c r="B93" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>42</v>
+      </c>
+      <c r="B97" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>42</v>
+      </c>
+      <c r="B98" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>42</v>
+      </c>
+      <c r="B99" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>102</v>
+      </c>
+      <c r="B101" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B105" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>102</v>
+      </c>
+      <c r="B106" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>102</v>
+      </c>
+      <c r="B108" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>102</v>
+      </c>
+      <c r="B109" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>102</v>
+      </c>
+      <c r="B110" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mejora de la base de datos, prueba de hiperparámetros
</commit_message>
<xml_diff>
--- a/chatbot/training_chatbot.xlsx
+++ b/chatbot/training_chatbot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataScience\Machine Learning\Projects\Keepcoding\TFB\TFB-SmartBot\chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B1C6C3-88B8-4EA4-A292-2A6DB79FB31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A22F3F7-46FA-4442-9D43-DA8DAC22160A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E701B219-9CB5-4FB1-A8B1-D6439049C12F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="119">
   <si>
     <t>Intent type</t>
   </si>
@@ -379,6 +379,21 @@
   </si>
   <si>
     <t>Cheerio</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>What can I do in this chatbot?</t>
+  </si>
+  <si>
+    <t>What options do I hace?</t>
+  </si>
+  <si>
+    <t>Tell me what can I ask for</t>
+  </si>
+  <si>
+    <t>Show me what you got</t>
   </si>
 </sst>
 </file>
@@ -730,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8947F2DF-9E18-4EF9-8E6E-53A318233C25}">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,6 +1636,38 @@
         <v>113</v>
       </c>
     </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>114</v>
+      </c>
+      <c r="B111" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>114</v>
+      </c>
+      <c r="B112" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>114</v>
+      </c>
+      <c r="B113" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>